<commit_message>
1008 US HK historical
</commit_message>
<xml_diff>
--- a/HK interest list.xlsx
+++ b/HK interest list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -504,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -694,12 +693,2273 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A452"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3968</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3908</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>6030</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>3993</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>6837</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>6881</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>6886</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>3888</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>6823</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>3883</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>7228</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>6169</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>6869</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>3898</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>6088</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>6068</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>3311</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>16852</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>8137</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>3377</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>3918</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>8227</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>3638</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>3669</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>7288</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>6818</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>8292</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>3606</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>7267</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>3933</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>6066</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>2638</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>6808</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>7321</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>6099</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>3339</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>8283</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>16823</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>3396</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>17081</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>8050</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>15733</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>7221</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>7388</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>6198</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>2868</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>17872</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>2662</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>8232</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>7341</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>8207</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>17898</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>6128</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>3969</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>3382</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>7230</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>